<commit_message>
with ngram correct data
</commit_message>
<xml_diff>
--- a/Test Data Per Error Type - Joey Tagged - Phrases.xlsx
+++ b/Test Data Per Error Type - Joey Tagged - Phrases.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Google Drive\Workspaces\Java\NGramChecker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37392" windowHeight="12588"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2597,7 +2592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2632,7 +2627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2843,16 +2838,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
@@ -2869,7 +2864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2883,7 +2878,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2897,7 +2892,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2911,7 +2906,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -2925,7 +2920,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2939,7 +2934,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2953,7 +2948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -2967,7 +2962,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2981,7 +2976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2995,7 +2990,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -3009,7 +3004,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -3037,7 +3032,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -3051,7 +3046,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -3065,7 +3060,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
@@ -3079,7 +3074,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3093,7 +3088,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -3107,7 +3102,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -3121,7 +3116,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -3135,7 +3130,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
@@ -3149,7 +3144,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -3163,7 +3158,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
@@ -3177,7 +3172,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
@@ -3191,7 +3186,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
@@ -3205,7 +3200,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -3219,7 +3214,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
@@ -3233,7 +3228,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
@@ -3261,7 +3256,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>62</v>
       </c>
@@ -3275,7 +3270,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>64</v>
       </c>
@@ -3289,7 +3284,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>66</v>
       </c>
@@ -3303,7 +3298,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
@@ -3317,7 +3312,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -3331,7 +3326,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>72</v>
       </c>
@@ -3345,7 +3340,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -3359,7 +3354,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>76</v>
       </c>
@@ -3373,7 +3368,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -3387,7 +3382,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>80</v>
       </c>
@@ -3401,7 +3396,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -3415,7 +3410,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
@@ -3429,7 +3424,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>86</v>
       </c>
@@ -3443,7 +3438,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>88</v>
       </c>
@@ -3457,7 +3452,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>90</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>92</v>
       </c>
@@ -3485,7 +3480,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>94</v>
       </c>
@@ -3499,7 +3494,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>96</v>
       </c>
@@ -3513,7 +3508,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>98</v>
       </c>
@@ -3527,7 +3522,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>100</v>
       </c>
@@ -3541,7 +3536,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>102</v>
       </c>
@@ -3555,7 +3550,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>140</v>
       </c>
@@ -3569,7 +3564,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>142</v>
       </c>
@@ -3583,7 +3578,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>144</v>
       </c>
@@ -3597,7 +3592,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>146</v>
       </c>
@@ -3611,7 +3606,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>148</v>
       </c>
@@ -3625,7 +3620,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>150</v>
       </c>
@@ -3639,7 +3634,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>151</v>
       </c>
@@ -3653,7 +3648,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>153</v>
       </c>
@@ -3667,7 +3662,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
@@ -3681,7 +3676,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>105</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>107</v>
       </c>
@@ -3709,7 +3704,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>529</v>
       </c>
@@ -3723,7 +3718,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>109</v>
       </c>
@@ -3737,7 +3732,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>111</v>
       </c>
@@ -3751,7 +3746,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>113</v>
       </c>
@@ -3765,7 +3760,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>115</v>
       </c>
@@ -3779,7 +3774,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>539</v>
       </c>
@@ -3793,7 +3788,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>117</v>
       </c>
@@ -3807,7 +3802,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>155</v>
       </c>
@@ -3821,7 +3816,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>157</v>
       </c>
@@ -3835,7 +3830,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>159</v>
       </c>
@@ -3849,7 +3844,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>160</v>
       </c>
@@ -3863,7 +3858,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
         <v>120</v>
       </c>
@@ -3877,7 +3872,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
         <v>122</v>
       </c>
@@ -3891,7 +3886,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>124</v>
       </c>
@@ -3905,7 +3900,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>162</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
         <v>164</v>
       </c>
@@ -3933,7 +3928,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
         <v>126</v>
       </c>
@@ -3947,7 +3942,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
         <v>166</v>
       </c>
@@ -3961,7 +3956,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
         <v>168</v>
       </c>
@@ -3975,7 +3970,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
         <v>128</v>
       </c>
@@ -3989,7 +3984,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
         <v>170</v>
       </c>
@@ -4003,7 +3998,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
         <v>172</v>
       </c>
@@ -4017,7 +4012,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
         <v>174</v>
       </c>
@@ -4031,7 +4026,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
         <v>176</v>
       </c>
@@ -4045,7 +4040,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>178</v>
       </c>
@@ -4059,7 +4054,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
         <v>180</v>
       </c>
@@ -4073,7 +4068,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>182</v>
       </c>
@@ -4087,7 +4082,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>184</v>
       </c>
@@ -4101,7 +4096,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
         <v>186</v>
       </c>
@@ -4115,7 +4110,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>188</v>
       </c>
@@ -4129,7 +4124,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>190</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>192</v>
       </c>
@@ -4157,7 +4152,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
         <v>130</v>
       </c>
@@ -4171,7 +4166,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>194</v>
       </c>
@@ -4185,7 +4180,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>196</v>
       </c>
@@ -4199,7 +4194,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
         <v>198</v>
       </c>
@@ -4213,7 +4208,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
         <v>132</v>
       </c>
@@ -4227,7 +4222,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
         <v>200</v>
       </c>
@@ -4241,7 +4236,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
         <v>202</v>
       </c>
@@ -4255,7 +4250,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
         <v>204</v>
       </c>
@@ -4269,7 +4264,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
         <v>206</v>
       </c>
@@ -4283,7 +4278,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
         <v>134</v>
       </c>
@@ -4297,7 +4292,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105" s="8" t="s">
         <v>136</v>
       </c>
@@ -4311,7 +4306,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
         <v>138</v>
       </c>
@@ -4325,7 +4320,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>208</v>
       </c>
@@ -4339,7 +4334,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>210</v>
       </c>
@@ -4353,7 +4348,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="11" t="s">
         <v>240</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="11" t="s">
         <v>617</v>
       </c>
@@ -4381,7 +4376,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="11" t="s">
         <v>243</v>
       </c>
@@ -4395,7 +4390,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="11" t="s">
         <v>245</v>
       </c>
@@ -4409,7 +4404,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="11" t="s">
         <v>247</v>
       </c>
@@ -4423,7 +4418,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
         <v>249</v>
       </c>
@@ -4437,7 +4432,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
         <v>251</v>
       </c>
@@ -4451,7 +4446,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="11" t="s">
         <v>253</v>
       </c>
@@ -4465,7 +4460,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="11" t="s">
         <v>255</v>
       </c>
@@ -4479,7 +4474,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
         <v>257</v>
       </c>
@@ -4493,7 +4488,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="11" t="s">
         <v>259</v>
       </c>
@@ -4507,7 +4502,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="11" t="s">
         <v>261</v>
       </c>
@@ -4521,7 +4516,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="11" t="s">
         <v>263</v>
       </c>
@@ -4535,7 +4530,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="11" t="s">
         <v>265</v>
       </c>
@@ -4549,7 +4544,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="11" t="s">
         <v>267</v>
       </c>
@@ -4563,7 +4558,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="11" t="s">
         <v>638</v>
       </c>
@@ -4577,7 +4572,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
         <v>269</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
         <v>212</v>
       </c>
@@ -4605,7 +4600,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
         <v>271</v>
       </c>
@@ -4619,7 +4614,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="11" t="s">
         <v>273</v>
       </c>
@@ -4633,7 +4628,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130" s="12" t="s">
         <v>275</v>
       </c>
@@ -4647,7 +4642,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131" s="11" t="s">
         <v>277</v>
       </c>
@@ -4661,7 +4656,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132" s="11" t="s">
         <v>279</v>
       </c>
@@ -4675,7 +4670,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A133" s="11" t="s">
         <v>281</v>
       </c>
@@ -4689,7 +4684,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134" s="11" t="s">
         <v>283</v>
       </c>
@@ -4703,7 +4698,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135" s="11" t="s">
         <v>285</v>
       </c>
@@ -4717,7 +4712,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136" s="11" t="s">
         <v>287</v>
       </c>
@@ -4731,7 +4726,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A137" s="11" t="s">
         <v>289</v>
       </c>
@@ -4745,7 +4740,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A138" s="11" t="s">
         <v>291</v>
       </c>
@@ -4759,7 +4754,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A139" s="11" t="s">
         <v>293</v>
       </c>
@@ -4773,7 +4768,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A140" s="11" t="s">
         <v>295</v>
       </c>
@@ -4787,7 +4782,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141" s="11" t="s">
         <v>297</v>
       </c>
@@ -4801,7 +4796,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142" s="12" t="s">
         <v>299</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A143" s="11" t="s">
         <v>214</v>
       </c>
@@ -4829,7 +4824,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A144" s="11" t="s">
         <v>301</v>
       </c>
@@ -4843,7 +4838,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A145" s="11" t="s">
         <v>303</v>
       </c>
@@ -4857,7 +4852,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A146" s="12" t="s">
         <v>305</v>
       </c>
@@ -4871,7 +4866,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A147" s="11" t="s">
         <v>216</v>
       </c>
@@ -4885,7 +4880,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
         <v>218</v>
       </c>
@@ -4899,7 +4894,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="11" t="s">
         <v>307</v>
       </c>
@@ -4913,7 +4908,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="11" t="s">
         <v>220</v>
       </c>
@@ -4927,7 +4922,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="11" t="s">
         <v>309</v>
       </c>
@@ -4941,7 +4936,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="11" t="s">
         <v>311</v>
       </c>
@@ -4955,7 +4950,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A153" s="11" t="s">
         <v>222</v>
       </c>
@@ -4969,7 +4964,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="11" t="s">
         <v>313</v>
       </c>
@@ -4983,7 +4978,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A155" s="11" t="s">
         <v>315</v>
       </c>
@@ -4997,7 +4992,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A156" s="11" t="s">
         <v>224</v>
       </c>
@@ -5011,7 +5006,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A157" s="11" t="s">
         <v>226</v>
       </c>
@@ -5025,7 +5020,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A158" s="11" t="s">
         <v>228</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="11" t="s">
         <v>317</v>
       </c>
@@ -5053,7 +5048,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A160" s="11" t="s">
         <v>319</v>
       </c>
@@ -5067,7 +5062,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A161" s="11" t="s">
         <v>321</v>
       </c>
@@ -5081,7 +5076,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A162" s="11" t="s">
         <v>706</v>
       </c>
@@ -5095,7 +5090,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A163" s="11" t="s">
         <v>323</v>
       </c>
@@ -5109,7 +5104,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A164" s="11" t="s">
         <v>325</v>
       </c>
@@ -5123,7 +5118,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A165" s="11" t="s">
         <v>327</v>
       </c>
@@ -5137,7 +5132,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="11" t="s">
         <v>329</v>
       </c>
@@ -5151,7 +5146,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="11" t="s">
         <v>230</v>
       </c>
@@ -5165,7 +5160,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="11" t="s">
         <v>331</v>
       </c>
@@ -5179,7 +5174,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="11" t="s">
         <v>333</v>
       </c>
@@ -5193,7 +5188,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="11" t="s">
         <v>232</v>
       </c>
@@ -5207,7 +5202,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="11" t="s">
         <v>234</v>
       </c>
@@ -5221,7 +5216,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="11" t="s">
         <v>335</v>
       </c>
@@ -5235,7 +5230,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="11" t="s">
         <v>337</v>
       </c>
@@ -5249,7 +5244,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="11" t="s">
         <v>339</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="11" t="s">
         <v>726</v>
       </c>
@@ -5277,7 +5272,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>341</v>
       </c>
@@ -5291,7 +5286,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
         <v>236</v>
       </c>
@@ -5305,7 +5300,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A178" s="11" t="s">
         <v>343</v>
       </c>
@@ -5319,7 +5314,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
         <v>345</v>
       </c>
@@ -5333,7 +5328,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A180" s="11" t="s">
         <v>347</v>
       </c>
@@ -5347,7 +5342,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
         <v>349</v>
       </c>
@@ -5361,7 +5356,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
         <v>351</v>
       </c>
@@ -5375,7 +5370,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A183" s="11" t="s">
         <v>353</v>
       </c>
@@ -5389,7 +5384,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A184" s="11" t="s">
         <v>355</v>
       </c>
@@ -5403,7 +5398,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A185" s="11" t="s">
         <v>357</v>
       </c>
@@ -5417,7 +5412,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A186" s="11" t="s">
         <v>359</v>
       </c>
@@ -5431,7 +5426,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A187" s="11" t="s">
         <v>361</v>
       </c>
@@ -5445,7 +5440,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A188" s="11" t="s">
         <v>363</v>
       </c>
@@ -5459,7 +5454,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A189" s="11" t="s">
         <v>365</v>
       </c>
@@ -5473,7 +5468,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A190" s="12" t="s">
         <v>367</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A191" s="11" t="s">
         <v>238</v>
       </c>
@@ -5501,7 +5496,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A192" s="11" t="s">
         <v>369</v>
       </c>
@@ -5515,7 +5510,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A193" s="11" t="s">
         <v>371</v>
       </c>
@@ -5529,7 +5524,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A194" s="11" t="s">
         <v>373</v>
       </c>
@@ -5543,7 +5538,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A195" s="11" t="s">
         <v>375</v>
       </c>
@@ -5557,7 +5552,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A196" s="11" t="s">
         <v>377</v>
       </c>
@@ -5571,7 +5566,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A197" s="11" t="s">
         <v>379</v>
       </c>
@@ -5585,7 +5580,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A198" s="11" t="s">
         <v>381</v>
       </c>
@@ -5599,7 +5594,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A199" s="11" t="s">
         <v>383</v>
       </c>
@@ -5613,7 +5608,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A200" s="11" t="s">
         <v>385</v>
       </c>
@@ -5627,7 +5622,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A201" s="11" t="s">
         <v>387</v>
       </c>
@@ -5641,7 +5636,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A202" s="11" t="s">
         <v>389</v>
       </c>
@@ -5655,7 +5650,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A203" s="12" t="s">
         <v>391</v>
       </c>
@@ -5669,7 +5664,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A204" s="11" t="s">
         <v>393</v>
       </c>
@@ -5683,7 +5678,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A205" s="11" t="s">
         <v>395</v>
       </c>
@@ -5697,7 +5692,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A207" s="13" t="s">
         <v>2</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A208" s="13" t="s">
         <v>397</v>
       </c>
@@ -5725,7 +5720,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A209" s="13" t="s">
         <v>105</v>
       </c>
@@ -5739,7 +5734,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A210" s="14" t="s">
         <v>399</v>
       </c>
@@ -5933,7 +5928,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5945,7 +5940,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>